<commit_message>
Last version of docs
</commit_message>
<xml_diff>
--- a/web_project_Scrum.xlsx
+++ b/web_project_Scrum.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krasm\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krasm\Downloads\Telegram Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D714D8C-82BB-4C5B-9D38-34A7AB8FFA58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D3ECFD-5B47-4289-B286-9915B3DDD941}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guide" sheetId="7" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="102">
   <si>
     <t>STATUS</t>
   </si>
@@ -36,30 +36,12 @@
     <t>User  Stroy</t>
   </si>
   <si>
-    <t xml:space="preserve">Spring Planning </t>
-  </si>
-  <si>
     <t>Participants</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Location </t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>Online</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>Story Point(s)</t>
   </si>
   <si>
@@ -147,21 +129,9 @@
     <t>Sprint Backlog : Sprint 2</t>
   </si>
   <si>
-    <t>19/03/2020</t>
-  </si>
-  <si>
     <t>N/R</t>
   </si>
   <si>
-    <t>Week 48</t>
-  </si>
-  <si>
-    <t>Week 49</t>
-  </si>
-  <si>
-    <t>Week 50</t>
-  </si>
-  <si>
     <t>STORY POINTS (NR)</t>
   </si>
   <si>
@@ -174,9 +144,6 @@
     <t>DEADLINE</t>
   </si>
   <si>
-    <t xml:space="preserve">As as a site visitor, I am able to navigate throught the website. </t>
-  </si>
-  <si>
     <t>As a site visitor with the mobile device, I should be able to use the web site not only on my laptop. (increase responisveness)</t>
   </si>
   <si>
@@ -195,9 +162,6 @@
     <t>Task: draw better background figure.</t>
   </si>
   <si>
-    <t xml:space="preserve">As a user, I should have easy-to-use and good-looking website. </t>
-  </si>
-  <si>
     <t>Task: Merge the css</t>
   </si>
   <si>
@@ -228,9 +192,6 @@
     <t>Task : Make a universal header + footer as a separate php file.</t>
   </si>
   <si>
-    <t>As a site visitor, I would like to have be able to observe the company not only on website, but also in other social media.</t>
-  </si>
-  <si>
     <t>Task: Add the contact us part in page (main?) + icons</t>
   </si>
   <si>
@@ -309,9 +270,6 @@
     <t xml:space="preserve">Maryna </t>
   </si>
   <si>
-    <t>As a web-site user , I would like to be able to observe the catalog of cars fully. (admin page)</t>
-  </si>
-  <si>
     <t>done</t>
   </si>
   <si>
@@ -319,13 +277,122 @@
   </si>
   <si>
     <t>Task: Design of contact us</t>
+  </si>
+  <si>
+    <t>As a site visitor, I would like to be able to observe the company not only on website, but also in other social media.</t>
+  </si>
+  <si>
+    <t>As as a site administrator, I would like to have a code that follows DRY (don't repeat yourself) criteria</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">User Story #1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>As as a site administrator, I would like to have a code that follows DRY (don't repeat yourself) criteria</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">User Story #2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>As a site visitor, I would like to be able to observe the company not only on website, but also in other social media.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">User Story #3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>As a site administrator, I woulld like to be able to administering the site's style in a single file</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">User Story #4 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>As a future customer of renting company, I should be able to choose dates when I want to rent a car.</t>
+    </r>
+  </si>
+  <si>
+    <t>As a site administrator, I would like to be able to manage the cars easily and display them to the user interface dynamically. (admin page)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">User Story #5 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>As a site administrator, I would like to be able to manage the cars easily and display them to the user interface dynamically. (admin page)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint Planning </t>
+  </si>
+  <si>
+    <t>Week 7</t>
+  </si>
+  <si>
+    <t>Week 8</t>
+  </si>
+  <si>
+    <t>Week 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Online </t>
+  </si>
+  <si>
+    <t>16/2/2021</t>
+  </si>
+  <si>
+    <t>22/2/2021</t>
+  </si>
+  <si>
+    <t>Week 10</t>
+  </si>
+  <si>
+    <t>28/2/2021</t>
+  </si>
+  <si>
+    <t>As a site administrator, I woulld like to be able to administering the site's style and content in a single file</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -428,6 +495,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -586,7 +659,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -617,6 +690,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2026,7 +2103,7 @@
   <sheetData>
     <row r="32" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M32" s="7" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="55" spans="10:18" x14ac:dyDescent="0.35">
@@ -2054,100 +2131,100 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95158496-5B07-4778-871C-839C6BA690D9}">
   <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView zoomScale="62" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="A4" zoomScale="77" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="80.58203125" customWidth="1"/>
-    <col min="2" max="2" width="21.75" customWidth="1"/>
-    <col min="3" max="3" width="20.25" customWidth="1"/>
-    <col min="4" max="4" width="22.75" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="79.5" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="33.5" x14ac:dyDescent="0.75">
-      <c r="A1" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="A1" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
     </row>
     <row r="2" spans="1:4" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>49</v>
+    <row r="3" spans="1:4" ht="34.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="16" t="s">
+        <v>85</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A4" s="16" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>56</v>
+    <row r="5" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="A5" s="16" t="s">
+        <v>101</v>
       </c>
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A11" s="16" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A12" s="16" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B12" s="2"/>
     </row>
@@ -2342,10 +2419,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABEC472C-4832-45AF-A950-04969A0E3C90}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2353,55 +2430,51 @@
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.08203125" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="26.75" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" customWidth="1"/>
     <col min="5" max="5" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>42</v>
+        <v>93</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>6</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
-        <v>40</v>
+      <c r="A4" s="19">
+        <v>44471</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2410,7 +2483,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>43</v>
+        <v>94</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
@@ -2419,20 +2492,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>10</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
-        <v>8</v>
+      <c r="A7" s="18" t="s">
+        <v>97</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2441,7 +2510,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -2450,25 +2519,48 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>10</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="8" t="s">
-        <v>8</v>
+      <c r="A10" s="18" t="s">
+        <v>98</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2480,72 +2572,72 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B586DF3-05CE-45CD-BBBF-F44EAB136942}">
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="84" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="38.83203125" customWidth="1"/>
-    <col min="2" max="2" width="11.75" customWidth="1"/>
-    <col min="3" max="3" width="13.25" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" customWidth="1"/>
-    <col min="10" max="10" width="12.75" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="28.5" x14ac:dyDescent="0.65">
-      <c r="A1" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-    </row>
-    <row r="2" spans="1:19" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+    </row>
+    <row r="2" spans="1:19" ht="25" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="K2" s="15"/>
       <c r="L2" s="15"/>
@@ -2557,9 +2649,9 @@
       <c r="R2" s="15"/>
       <c r="S2" s="15"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="13"/>
@@ -2582,13 +2674,13 @@
     </row>
     <row r="4" spans="1:19" ht="25" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
@@ -2611,13 +2703,13 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
@@ -2638,9 +2730,9 @@
       <c r="R5" s="15"/>
       <c r="S5" s="15"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
-        <v>24</v>
+        <v>87</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="13"/>
@@ -2663,13 +2755,13 @@
     </row>
     <row r="7" spans="1:19" ht="25" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
@@ -2692,13 +2784,13 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
@@ -2721,13 +2813,13 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -2750,13 +2842,13 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
@@ -2779,13 +2871,13 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
@@ -2806,9 +2898,9 @@
       <c r="R11" s="15"/>
       <c r="S11" s="15"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
-        <v>25</v>
+        <v>88</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
@@ -2831,11 +2923,11 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="14" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
@@ -2856,9 +2948,9 @@
       <c r="R13" s="15"/>
       <c r="S13" s="15"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:19" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
-        <v>26</v>
+        <v>89</v>
       </c>
       <c r="B14" s="12"/>
       <c r="C14" s="13"/>
@@ -2881,13 +2973,13 @@
     </row>
     <row r="15" spans="1:19" ht="25" x14ac:dyDescent="0.35">
       <c r="A15" s="14" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
@@ -2908,9 +3000,9 @@
       <c r="R15" s="15"/>
       <c r="S15" s="15"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:19" ht="50" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
-        <v>27</v>
+        <v>91</v>
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="13"/>
@@ -2933,13 +3025,13 @@
     </row>
     <row r="17" spans="1:19" ht="25" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
@@ -2962,13 +3054,13 @@
     </row>
     <row r="18" spans="1:19" ht="25" x14ac:dyDescent="0.35">
       <c r="A18" s="14" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
@@ -2991,7 +3083,7 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -3032,7 +3124,7 @@
     <mergeCell ref="A1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3040,68 +3132,68 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6493C1AE-7DEA-468D-A29A-77DFE72F7817}">
   <dimension ref="A1:S24"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="92" workbookViewId="0">
+    <sheetView zoomScale="92" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="38.83203125" customWidth="1"/>
-    <col min="2" max="2" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.25" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="28.5" x14ac:dyDescent="0.65">
-      <c r="A1" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
+      <c r="A1" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
     </row>
     <row r="2" spans="1:19" ht="25" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="J2" s="15"/>
       <c r="K2" s="15"/>
@@ -3116,7 +3208,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="13"/>
@@ -3139,11 +3231,11 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="14" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
@@ -3164,11 +3256,11 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B5" s="14"/>
       <c r="C5" s="14" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
@@ -3189,11 +3281,11 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="B6" s="14"/>
       <c r="C6" s="14" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
@@ -3214,11 +3306,11 @@
     </row>
     <row r="7" spans="1:19" ht="25" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="14" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
@@ -3239,7 +3331,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="13"/>
@@ -3262,11 +3354,11 @@
     </row>
     <row r="9" spans="1:19" ht="25" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="14" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -3287,11 +3379,11 @@
     </row>
     <row r="10" spans="1:19" ht="25" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="14" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
@@ -3312,11 +3404,11 @@
     </row>
     <row r="11" spans="1:19" ht="25" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="14" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
@@ -3337,11 +3429,11 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B12" s="14"/>
       <c r="C12" s="14" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
@@ -3362,11 +3454,11 @@
     </row>
     <row r="13" spans="1:19" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="14" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
@@ -3387,11 +3479,11 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" s="14" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B14" s="14"/>
       <c r="C14" s="14" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
@@ -3412,7 +3504,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="13"/>
@@ -3435,11 +3527,11 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="B16" s="14"/>
       <c r="C16" s="14" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
@@ -3460,7 +3552,7 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="B17" s="12"/>
       <c r="C17" s="13"/>
@@ -3483,11 +3575,11 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A18" s="14" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="B18" s="14"/>
       <c r="C18" s="14" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
@@ -3508,11 +3600,11 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A19" s="14" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="B19" s="14"/>
       <c r="C19" s="14" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
@@ -3533,11 +3625,11 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A20" s="14" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="B20" s="14"/>
       <c r="C20" s="14" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
@@ -3558,11 +3650,11 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A21" s="14" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="B21" s="14"/>
       <c r="C21" s="14" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
@@ -3583,7 +3675,7 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="13"/>
@@ -3606,11 +3698,11 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A23" s="14" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B23" s="14"/>
       <c r="C23" s="14" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
@@ -3631,7 +3723,7 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
@@ -3686,61 +3778,61 @@
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="38.83203125" customWidth="1"/>
-    <col min="2" max="2" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.25" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="28.5" x14ac:dyDescent="0.65">
-      <c r="A1" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
+      <c r="A1" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
     </row>
     <row r="2" spans="1:19" ht="25" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="J2" s="15"/>
       <c r="K2" s="15"/>
@@ -3755,7 +3847,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="13"/>
@@ -3778,16 +3870,16 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B4" s="14">
         <v>2</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E4" s="14">
         <v>2</v>
@@ -3817,13 +3909,13 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B5" s="14">
         <v>2</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="14">
@@ -3854,13 +3946,13 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B6" s="14">
         <v>4</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="14">
@@ -3891,13 +3983,13 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B7" s="14">
         <v>2</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="14">
@@ -3928,7 +4020,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="13"/>
@@ -3951,7 +4043,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
@@ -3974,7 +4066,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
@@ -3997,7 +4089,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
@@ -4020,7 +4112,7 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
@@ -4043,7 +4135,7 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="13"/>
@@ -4066,7 +4158,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -4089,7 +4181,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" s="14" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
@@ -4112,7 +4204,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
@@ -4135,7 +4227,7 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
@@ -4158,7 +4250,7 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="13"/>
@@ -4181,7 +4273,7 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A19" s="14" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
@@ -4204,7 +4296,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A20" s="14" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
@@ -4227,7 +4319,7 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A21" s="14" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
@@ -4250,7 +4342,7 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A22" s="14" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
@@ -4273,7 +4365,7 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A23" s="12" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="13"/>
@@ -4296,7 +4388,7 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A24" s="14" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
@@ -4319,7 +4411,7 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A25" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
@@ -4342,7 +4434,7 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A26" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
@@ -4365,7 +4457,7 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A27" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
@@ -4388,7 +4480,7 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A28" s="10" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>

</xml_diff>